<commit_message>
Updated main Cstock figure with detailed C-N values
</commit_message>
<xml_diff>
--- a/DATA/C-N.xlsx
+++ b/DATA/C-N.xlsx
@@ -3395,6 +3395,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3716,8 +3720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56863C3-93C9-42B6-878D-C24BE69AB489}">
   <dimension ref="A1:N763"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A717" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E719" sqref="E719"/>
+    <sheetView tabSelected="1" topLeftCell="A709" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E709" sqref="E709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>